<commit_message>
Alteração do layout de impressão para paisagem.
</commit_message>
<xml_diff>
--- a/Horas Trabalhadas.xlsx
+++ b/Horas Trabalhadas.xlsx
@@ -457,11 +457,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41:M41"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1794,8 +1797,8 @@
       <c r="G42" s="12"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="81" orientation="landscape" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Atualização; Inclusão da lista de ignorados.
</commit_message>
<xml_diff>
--- a/Horas Trabalhadas.xlsx
+++ b/Horas Trabalhadas.xlsx
@@ -83,7 +83,7 @@
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
     <numFmt numFmtId="165" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +112,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +138,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -170,12 +182,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -187,7 +215,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="22" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -201,8 +228,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2"/>
+    <xf numFmtId="22" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Entrada" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -504,11 +539,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,31 +564,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -750,161 +785,161 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="3">
+      <c r="A8" s="12">
         <v>39826.365972222222</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12">
         <v>39826.90625</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14">
         <v>39826.5</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="3">
+      <c r="F8" s="14"/>
+      <c r="G8" s="12">
         <v>39826.541666666664</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5">
+      <c r="H8" s="13"/>
+      <c r="I8" s="15">
         <f t="shared" si="1"/>
         <v>0.5819444444423425</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6">
+      <c r="J8" s="13"/>
+      <c r="K8" s="16">
         <f t="shared" si="2"/>
         <v>0.24861111110900919</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4" t="str">
+      <c r="L8" s="13"/>
+      <c r="M8" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="3">
+      <c r="A9" s="12">
         <v>39827.370833333334</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12">
         <v>39827.512499999997</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3">
+      <c r="D9" s="13"/>
+      <c r="E9" s="12">
         <v>39827.555555555555</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12">
         <v>39827.847916666666</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5">
+      <c r="H9" s="13"/>
+      <c r="I9" s="15">
         <f t="shared" si="1"/>
         <v>0.43402777777373558</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="6">
+      <c r="J9" s="13"/>
+      <c r="K9" s="16">
         <f t="shared" si="2"/>
         <v>0.10069444444040226</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4" t="str">
+      <c r="L9" s="13"/>
+      <c r="M9" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="3">
+      <c r="A10" s="12">
         <v>39828.382638888892</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12">
         <v>39828.505555555559</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3">
+      <c r="D10" s="13"/>
+      <c r="E10" s="12">
         <v>39828.59375</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12">
         <v>39828.824999999997</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5">
+      <c r="H10" s="13"/>
+      <c r="I10" s="15">
         <f t="shared" si="1"/>
         <v>0.35416666666424135</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="6">
+      <c r="J10" s="13"/>
+      <c r="K10" s="16">
         <f t="shared" si="2"/>
         <v>2.0833333330908033E-2</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4" t="str">
+      <c r="L10" s="13"/>
+      <c r="M10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="3">
+      <c r="A11" s="12">
         <v>39829.338194444441</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12">
         <v>39829.509722222225</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3">
+      <c r="D11" s="13"/>
+      <c r="E11" s="12">
         <v>39829.551388888889</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12">
         <v>39829.724999999999</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5">
+      <c r="H11" s="13"/>
+      <c r="I11" s="15">
         <f t="shared" si="1"/>
         <v>0.34513888889341615</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="6">
+      <c r="J11" s="13"/>
+      <c r="K11" s="16">
         <f t="shared" si="2"/>
         <v>1.1805555560082837E-2</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4" t="str">
+      <c r="L11" s="13"/>
+      <c r="M11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="3">
+      <c r="A12" s="12">
         <v>39830.427083333336</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12">
         <v>39830.526388888888</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3">
+      <c r="D12" s="13"/>
+      <c r="E12" s="12">
         <v>39830.606944444444</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3">
+      <c r="F12" s="12"/>
+      <c r="G12" s="12">
         <v>39830.848611111112</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5">
+      <c r="H12" s="13"/>
+      <c r="I12" s="15">
         <f t="shared" si="1"/>
         <v>0.34097222222044365</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="6">
+      <c r="J12" s="13"/>
+      <c r="K12" s="16">
         <f t="shared" si="2"/>
         <v>7.63888888711034E-3</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4" t="str">
+      <c r="L12" s="13"/>
+      <c r="M12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Sexta</v>
       </c>
@@ -1038,161 +1073,161 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="3">
+      <c r="A17" s="12">
         <v>39840.406944444447</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12">
         <v>39840.520138888889</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3">
+      <c r="D17" s="13"/>
+      <c r="E17" s="12">
         <v>39840.565972222219</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12">
         <v>39840.824305555558</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5">
+      <c r="H17" s="13"/>
+      <c r="I17" s="15">
         <f t="shared" si="1"/>
         <v>0.37152777778101154</v>
       </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="6">
+      <c r="J17" s="13"/>
+      <c r="K17" s="16">
         <f t="shared" si="2"/>
         <v>3.8194444447678222E-2</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4" t="str">
+      <c r="L17" s="13"/>
+      <c r="M17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="3">
+      <c r="A18" s="12">
         <v>39841.382638888892</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12">
         <v>39841.50277777778</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3">
+      <c r="D18" s="13"/>
+      <c r="E18" s="12">
         <v>39841.536805555559</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12">
         <v>39841.789583333331</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5">
+      <c r="H18" s="13"/>
+      <c r="I18" s="15">
         <f t="shared" si="1"/>
         <v>0.37291666665987577</v>
       </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="6">
+      <c r="J18" s="13"/>
+      <c r="K18" s="16">
         <f t="shared" si="2"/>
         <v>3.9583333326542458E-2</v>
       </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4" t="str">
+      <c r="L18" s="13"/>
+      <c r="M18" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="3">
+      <c r="A19" s="12">
         <v>39842.39166666667</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12">
         <v>39842.515277777777</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3">
+      <c r="D19" s="13"/>
+      <c r="E19" s="12">
         <v>39842.566666666666</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3">
+      <c r="F19" s="12"/>
+      <c r="G19" s="12">
         <v>39842.833333333336</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5">
+      <c r="H19" s="13"/>
+      <c r="I19" s="15">
         <f t="shared" si="1"/>
         <v>0.39027777777664596</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="6">
+      <c r="J19" s="13"/>
+      <c r="K19" s="16">
         <f t="shared" si="2"/>
         <v>5.6944444443312647E-2</v>
       </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4" t="str">
+      <c r="L19" s="13"/>
+      <c r="M19" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="3">
+      <c r="A20" s="12">
         <v>39843.397916666669</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12">
         <v>39843.507638888892</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3">
+      <c r="D20" s="13"/>
+      <c r="E20" s="12">
         <v>39843.577777777777</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3">
+      <c r="F20" s="12"/>
+      <c r="G20" s="12">
         <v>39843.760416666664</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5">
+      <c r="H20" s="13"/>
+      <c r="I20" s="15">
         <f t="shared" si="1"/>
         <v>0.29236111111094942</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="6">
+      <c r="J20" s="13"/>
+      <c r="K20" s="16">
         <f t="shared" si="2"/>
         <v>-4.0972222222383892E-2</v>
       </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4" t="str">
+      <c r="L20" s="13"/>
+      <c r="M20" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="3">
+      <c r="A21" s="12">
         <v>39844.337500000001</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12">
         <v>39844.520138888889</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3">
+      <c r="D21" s="13"/>
+      <c r="E21" s="12">
         <v>39844.566666666666</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3">
+      <c r="F21" s="12"/>
+      <c r="G21" s="12">
         <v>39844.729861111111</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5">
+      <c r="H21" s="13"/>
+      <c r="I21" s="15">
         <f t="shared" si="1"/>
         <v>0.34583333333284827</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="6">
+      <c r="J21" s="13"/>
+      <c r="K21" s="16">
         <f t="shared" si="2"/>
         <v>1.2499999999514955E-2</v>
       </c>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4" t="str">
+      <c r="L21" s="13"/>
+      <c r="M21" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Sexta</v>
       </c>
@@ -1294,27 +1329,27 @@
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>39850.400000000001</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="10">
+      <c r="B25" s="10"/>
+      <c r="C25" s="9">
         <v>39850.506944444445</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="10">
+      <c r="D25" s="10"/>
+      <c r="E25" s="9">
         <v>39850.548611111109</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="10">
+      <c r="F25" s="10"/>
+      <c r="G25" s="9">
         <v>39850.774305555555</v>
       </c>
-      <c r="H25" s="11"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="5">
         <f t="shared" si="1"/>
         <v>0.33263888888905058</v>
       </c>
-      <c r="J25" s="11"/>
+      <c r="J25" s="10"/>
       <c r="K25" s="6">
         <f t="shared" ref="K25" si="3">IF(OR(WEEKDAY(A25)=7,WEEKDAY(A25)=1),I25,I25-"08:00:00")</f>
         <v>-6.9444444428273799E-4</v>
@@ -1326,1365 +1361,1653 @@
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>39851.35</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="10">
+      <c r="B26" s="10"/>
+      <c r="C26" s="9">
         <v>39851.538194444445</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="10">
+      <c r="D26" s="10"/>
+      <c r="E26" s="9">
         <v>39851.579861111109</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10">
+      <c r="F26" s="10"/>
+      <c r="G26" s="9">
         <v>39851.729861111111</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="5">
         <f t="shared" si="1"/>
         <v>0.33819444444816327</v>
       </c>
-      <c r="J26" s="11"/>
+      <c r="J26" s="10"/>
       <c r="K26" s="6">
         <f t="shared" ref="K26:K32" si="5">IF(OR(WEEKDAY(A26)=7,WEEKDAY(A26)=1),I26,I26-"08:00:00")</f>
         <v>4.8611111148299524E-3</v>
       </c>
-      <c r="L26" s="11"/>
+      <c r="L26" s="10"/>
       <c r="M26" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Sexta</v>
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="10">
+      <c r="A27" s="12">
         <v>39854</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="6">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="16">
         <f t="shared" si="5"/>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="L27" s="11"/>
-      <c r="M27" s="4" t="str">
+      <c r="L27" s="13"/>
+      <c r="M27" s="13" t="str">
         <f t="shared" si="4"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="10">
+      <c r="A28" s="12">
         <v>39856.409722222219</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="10">
+      <c r="B28" s="13"/>
+      <c r="C28" s="12">
         <v>39856.496527777781</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10">
+      <c r="D28" s="13"/>
+      <c r="E28" s="12">
         <v>39856.536805555559</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="10">
+      <c r="F28" s="13"/>
+      <c r="G28" s="12">
         <v>39856.788888888892</v>
       </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="5">
+      <c r="H28" s="13"/>
+      <c r="I28" s="15">
         <f t="shared" si="1"/>
         <v>0.33888888889487134</v>
       </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="6">
+      <c r="J28" s="13"/>
+      <c r="K28" s="16">
         <f t="shared" si="5"/>
         <v>5.5555555615380281E-3</v>
       </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="4" t="str">
+      <c r="L28" s="13"/>
+      <c r="M28" s="13" t="str">
         <f t="shared" si="4"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="10">
+      <c r="A29" s="12">
         <v>39857.395833333336</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="10">
+      <c r="B29" s="13"/>
+      <c r="C29" s="12">
         <v>39857.518055555556</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="10">
+      <c r="D29" s="13"/>
+      <c r="E29" s="12">
         <v>39857.550694444442</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="10">
+      <c r="F29" s="13"/>
+      <c r="G29" s="12">
         <v>39857.786805555559</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="5">
+      <c r="H29" s="13"/>
+      <c r="I29" s="15">
         <f t="shared" si="1"/>
         <v>0.35833333333721384</v>
       </c>
-      <c r="J29" s="11"/>
-      <c r="K29" s="6">
+      <c r="J29" s="13"/>
+      <c r="K29" s="16">
         <f t="shared" si="5"/>
         <v>2.5000000003880529E-2</v>
       </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="4" t="str">
+      <c r="L29" s="13"/>
+      <c r="M29" s="13" t="str">
         <f t="shared" si="4"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="10">
+      <c r="A30" s="12">
         <v>39858.341666666667</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="10">
+      <c r="B30" s="13"/>
+      <c r="C30" s="12">
         <v>39858.536805555559</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="10">
+      <c r="D30" s="13"/>
+      <c r="E30" s="12">
         <v>39858.586111111108</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="10">
+      <c r="F30" s="13"/>
+      <c r="G30" s="12">
         <v>39858.729166666664</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="5">
+      <c r="H30" s="13"/>
+      <c r="I30" s="15">
         <f>(G30-E30)+(C30-A30)</f>
         <v>0.33819444444816327</v>
       </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="6">
+      <c r="J30" s="13"/>
+      <c r="K30" s="16">
         <f t="shared" si="5"/>
         <v>4.8611111148299524E-3</v>
       </c>
-      <c r="L30" s="11"/>
-      <c r="M30" s="4" t="str">
+      <c r="L30" s="13"/>
+      <c r="M30" s="13" t="str">
         <f t="shared" si="4"/>
         <v>Sexta</v>
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="10">
+      <c r="A31" s="9">
         <v>39861.387499999997</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="10">
+      <c r="B31" s="10"/>
+      <c r="C31" s="9">
         <v>39861.513194444444</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="10">
+      <c r="D31" s="10"/>
+      <c r="E31" s="9">
         <v>39861.563888888886</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="10">
+      <c r="F31" s="10"/>
+      <c r="G31" s="9">
         <v>39861.868750000001</v>
       </c>
-      <c r="H31" s="11"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="5">
         <f>(G31-E31)+(C31-A31)</f>
         <v>0.43055555556202307</v>
       </c>
-      <c r="J31" s="11"/>
+      <c r="J31" s="10"/>
       <c r="K31" s="6">
         <f t="shared" si="5"/>
         <v>9.7222222228689759E-2</v>
       </c>
-      <c r="L31" s="11"/>
+      <c r="L31" s="10"/>
       <c r="M31" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="10">
+      <c r="A32" s="9">
         <v>39862.400694444441</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="10">
+      <c r="B32" s="10"/>
+      <c r="C32" s="9">
         <v>39862.509027777778</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="10">
+      <c r="D32" s="10"/>
+      <c r="E32" s="9">
         <v>39862.554861111108</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="10">
+      <c r="F32" s="10"/>
+      <c r="G32" s="9">
         <v>39862.804166666669</v>
       </c>
-      <c r="H32" s="11"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="5">
         <f>(G32-E32)+(C32-A32)</f>
         <v>0.35763888889778173</v>
       </c>
-      <c r="J32" s="11"/>
+      <c r="J32" s="10"/>
       <c r="K32" s="6">
         <f t="shared" si="5"/>
         <v>2.4305555564448411E-2</v>
       </c>
-      <c r="L32" s="11"/>
+      <c r="L32" s="10"/>
       <c r="M32" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>39863.402083333334</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="10">
+      <c r="B33" s="10"/>
+      <c r="C33" s="9">
         <v>39863.495833333334</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="10">
+      <c r="D33" s="10"/>
+      <c r="E33" s="9">
         <v>39863.54583333333</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="10">
+      <c r="F33" s="10"/>
+      <c r="G33" s="9">
         <v>39863.89166666667</v>
       </c>
-      <c r="H33" s="11"/>
+      <c r="H33" s="10"/>
       <c r="I33" s="5">
         <f t="shared" ref="I33:I34" si="6">(G33-E33)+(C33-A33)</f>
         <v>0.43958333334012423</v>
       </c>
-      <c r="J33" s="11"/>
+      <c r="J33" s="10"/>
       <c r="K33" s="6">
         <f t="shared" ref="K33:K34" si="7">IF(OR(WEEKDAY(A33)=7,WEEKDAY(A33)=1),I33,I33-"08:00:00")</f>
         <v>0.10625000000679091</v>
       </c>
-      <c r="L33" s="11"/>
+      <c r="L33" s="10"/>
       <c r="M33" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <v>39864.402083333334</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10">
+      <c r="B34" s="10"/>
+      <c r="C34" s="9">
         <v>39864.504166666666</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="10">
+      <c r="D34" s="10"/>
+      <c r="E34" s="9">
         <v>39864.572916666664</v>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="10">
+      <c r="F34" s="10"/>
+      <c r="G34" s="9">
         <v>39864.885416666664</v>
       </c>
-      <c r="H34" s="11"/>
+      <c r="H34" s="10"/>
       <c r="I34" s="5">
         <f t="shared" si="6"/>
         <v>0.41458333333139308</v>
       </c>
-      <c r="J34" s="11"/>
+      <c r="J34" s="10"/>
       <c r="K34" s="6">
         <f t="shared" si="7"/>
         <v>8.1249999998059763E-2</v>
       </c>
-      <c r="L34" s="11"/>
+      <c r="L34" s="10"/>
       <c r="M34" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="10">
+      <c r="A35" s="9">
         <v>39865.388194444444</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10">
+      <c r="B35" s="10"/>
+      <c r="C35" s="9">
         <v>39865.521527777775</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="10">
+      <c r="D35" s="10"/>
+      <c r="E35" s="9">
         <v>39865.583333333336</v>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="10">
+      <c r="F35" s="10"/>
+      <c r="G35" s="9">
         <v>39865.804166666669</v>
       </c>
-      <c r="H35" s="11"/>
+      <c r="H35" s="10"/>
       <c r="I35" s="5">
         <f>(G35-E35)+(C35-A35)</f>
         <v>0.35416666666424135</v>
       </c>
-      <c r="J35" s="11"/>
+      <c r="J35" s="10"/>
       <c r="K35" s="6">
         <f>IF(OR(WEEKDAY(A35)=7,WEEKDAY(A35)=1),I35,I35-"08:00:00")</f>
         <v>2.0833333330908033E-2</v>
       </c>
-      <c r="L35" s="11"/>
+      <c r="L35" s="10"/>
       <c r="M35" s="4" t="str">
         <f>IF(WEEKDAY(A35)=1,"Domingo",IF(WEEKDAY(A35)=2,"Segunda",IF(WEEKDAY(A35)=3,"Terça",IF(WEEKDAY(A35)=4,"Quarta",IF(WEEKDAY(A35)=5,"Quinta",IF(WEEKDAY(A35)=6,"Sexta",IF(WEEKDAY(A35)=7,"Sábado","Domingo")))))))</f>
         <v>Sexta</v>
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="10">
+      <c r="A36" s="12">
         <v>39868.347916666666</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="10">
+      <c r="B36" s="13"/>
+      <c r="C36" s="12">
         <v>39868.515972222223</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="10">
+      <c r="D36" s="13"/>
+      <c r="E36" s="12">
         <v>39868.568055555559</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="10">
+      <c r="F36" s="13"/>
+      <c r="G36" s="12">
         <v>39868.793055555558</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="5">
+      <c r="H36" s="13"/>
+      <c r="I36" s="15">
         <f>(G36-E36)+(C36-A36)</f>
         <v>0.39305555555620231</v>
       </c>
-      <c r="J36" s="11"/>
-      <c r="K36" s="6">
+      <c r="J36" s="13"/>
+      <c r="K36" s="16">
         <f>IF(OR(WEEKDAY(A36)=7,WEEKDAY(A36)=1),I36,I36-"08:00:00")</f>
         <v>5.9722222222868993E-2</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="4" t="str">
+      <c r="L36" s="13"/>
+      <c r="M36" s="13" t="str">
         <f>IF(WEEKDAY(A36)=1,"Domingo",IF(WEEKDAY(A36)=2,"Segunda",IF(WEEKDAY(A36)=3,"Terça",IF(WEEKDAY(A36)=4,"Quarta",IF(WEEKDAY(A36)=5,"Quinta",IF(WEEKDAY(A36)=6,"Sexta",IF(WEEKDAY(A36)=7,"Sábado","Domingo")))))))</f>
         <v>Segunda</v>
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="10">
+      <c r="A37" s="12">
         <v>39869.368750000001</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="10">
+      <c r="B37" s="13"/>
+      <c r="C37" s="12">
         <v>39869.52847222222</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="10">
+      <c r="D37" s="13"/>
+      <c r="E37" s="12">
         <v>39869.581250000003</v>
       </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="10">
+      <c r="F37" s="13"/>
+      <c r="G37" s="12">
         <v>39869.84097222222</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="5">
+      <c r="H37" s="13"/>
+      <c r="I37" s="15">
         <f t="shared" ref="I37:I53" si="8">(G37-E37)+(C37-A37)</f>
         <v>0.41944444443652174</v>
       </c>
-      <c r="J37" s="11"/>
-      <c r="K37" s="6">
+      <c r="J37" s="13"/>
+      <c r="K37" s="16">
         <f t="shared" ref="K37:K53" si="9">IF(OR(WEEKDAY(A37)=7,WEEKDAY(A37)=1),I37,I37-"08:00:00")</f>
         <v>8.611111110318842E-2</v>
       </c>
-      <c r="L37" s="11"/>
-      <c r="M37" s="4" t="str">
+      <c r="L37" s="13"/>
+      <c r="M37" s="13" t="str">
         <f t="shared" ref="M37:M53" si="10">IF(WEEKDAY(A37)=1,"Domingo",IF(WEEKDAY(A37)=2,"Segunda",IF(WEEKDAY(A37)=3,"Terça",IF(WEEKDAY(A37)=4,"Quarta",IF(WEEKDAY(A37)=5,"Quinta",IF(WEEKDAY(A37)=6,"Sexta",IF(WEEKDAY(A37)=7,"Sábado","Domingo")))))))</f>
         <v>Terça</v>
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="10">
+      <c r="A38" s="12">
         <v>39870.415277777778</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="10">
+      <c r="B38" s="13"/>
+      <c r="C38" s="12">
         <v>39870.541666666664</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="10">
+      <c r="D38" s="13"/>
+      <c r="E38" s="12">
         <v>39870.589583333334</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="10">
+      <c r="F38" s="13"/>
+      <c r="G38" s="12">
         <v>39870.865277777775</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="5">
+      <c r="H38" s="13"/>
+      <c r="I38" s="15">
         <f t="shared" si="8"/>
         <v>0.4020833333270275</v>
       </c>
-      <c r="J38" s="11"/>
-      <c r="K38" s="6">
+      <c r="J38" s="13"/>
+      <c r="K38" s="16">
         <f t="shared" si="9"/>
         <v>6.8749999993694189E-2</v>
       </c>
-      <c r="L38" s="11"/>
-      <c r="M38" s="4" t="str">
+      <c r="L38" s="13"/>
+      <c r="M38" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="10">
+      <c r="A39" s="12">
         <v>39871.40902777778</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="10">
+      <c r="B39" s="13"/>
+      <c r="C39" s="12">
         <v>39871.527083333334</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="10">
+      <c r="D39" s="13"/>
+      <c r="E39" s="12">
         <v>39871.601388888892</v>
       </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="10">
+      <c r="F39" s="13"/>
+      <c r="G39" s="12">
         <v>39871.892361111109</v>
       </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="5">
+      <c r="H39" s="13"/>
+      <c r="I39" s="15">
         <f t="shared" si="8"/>
         <v>0.40902777777228039</v>
       </c>
-      <c r="J39" s="11"/>
-      <c r="K39" s="6">
+      <c r="J39" s="13"/>
+      <c r="K39" s="16">
         <f t="shared" si="9"/>
         <v>7.5694444438947073E-2</v>
       </c>
-      <c r="L39" s="11"/>
-      <c r="M39" s="4" t="str">
+      <c r="L39" s="13"/>
+      <c r="M39" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="10">
+      <c r="A40" s="12">
         <v>39872.336805555555</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="10">
+      <c r="B40" s="13"/>
+      <c r="C40" s="12">
         <v>39872.510416666664</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="10">
+      <c r="D40" s="13"/>
+      <c r="E40" s="12">
         <v>39872.563194444447</v>
       </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="10">
+      <c r="F40" s="13"/>
+      <c r="G40" s="12">
         <v>39872.697916666664</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="5">
+      <c r="H40" s="13"/>
+      <c r="I40" s="15">
         <f t="shared" si="8"/>
         <v>0.3083333333270275</v>
       </c>
-      <c r="J40" s="11"/>
-      <c r="K40" s="6">
+      <c r="J40" s="13"/>
+      <c r="K40" s="16">
         <f t="shared" si="9"/>
         <v>-2.5000000006305811E-2</v>
       </c>
-      <c r="L40" s="11"/>
-      <c r="M40" s="4" t="str">
+      <c r="L40" s="13"/>
+      <c r="M40" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Sexta</v>
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="10">
+      <c r="A41" s="9">
         <v>39875.369444444441</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="10">
+      <c r="B41" s="10"/>
+      <c r="C41" s="9">
         <v>39875.522222222222</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="10">
+      <c r="D41" s="10"/>
+      <c r="E41" s="9">
         <v>39875.574305555558</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="10">
+      <c r="F41" s="10"/>
+      <c r="G41" s="9">
         <v>39875.88958333333</v>
       </c>
-      <c r="H41" s="11"/>
+      <c r="H41" s="10"/>
       <c r="I41" s="5">
         <f t="shared" si="8"/>
         <v>0.46805555555329192</v>
       </c>
-      <c r="J41" s="11"/>
+      <c r="J41" s="10"/>
       <c r="K41" s="6">
         <f t="shared" si="9"/>
         <v>0.13472222221995861</v>
       </c>
-      <c r="L41" s="11"/>
+      <c r="L41" s="10"/>
       <c r="M41" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="10">
+      <c r="A42" s="9">
         <v>39876.338194444441</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10">
+      <c r="B42" s="10"/>
+      <c r="C42" s="9">
         <v>39876.513194444444</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10">
+      <c r="D42" s="10"/>
+      <c r="E42" s="9">
         <v>39876.561805555553</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="10">
+      <c r="F42" s="10"/>
+      <c r="G42" s="9">
         <v>39876.834722222222</v>
       </c>
-      <c r="H42" s="11"/>
+      <c r="H42" s="10"/>
       <c r="I42" s="5">
         <f t="shared" si="8"/>
         <v>0.44791666667151731</v>
       </c>
-      <c r="J42" s="11"/>
+      <c r="J42" s="10"/>
       <c r="K42" s="6">
         <f t="shared" si="9"/>
         <v>0.11458333333818399</v>
       </c>
-      <c r="L42" s="11"/>
+      <c r="L42" s="10"/>
       <c r="M42" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="10">
+      <c r="A43" s="9">
         <v>39877.395138888889</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="10">
+      <c r="B43" s="10"/>
+      <c r="C43" s="9">
         <v>39877.527777777781</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="10">
+      <c r="D43" s="10"/>
+      <c r="E43" s="9">
         <v>39877.579861111109</v>
       </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="10">
+      <c r="F43" s="10"/>
+      <c r="G43" s="9">
         <v>39877.790972222225</v>
       </c>
-      <c r="H43" s="11"/>
+      <c r="H43" s="10"/>
       <c r="I43" s="5">
         <f t="shared" si="8"/>
         <v>0.34375000000727596</v>
       </c>
-      <c r="J43" s="11"/>
+      <c r="J43" s="10"/>
       <c r="K43" s="6">
         <f t="shared" si="9"/>
         <v>1.0416666673942643E-2</v>
       </c>
-      <c r="L43" s="11"/>
+      <c r="L43" s="10"/>
       <c r="M43" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="10">
+      <c r="A44" s="9">
         <v>39878.407638888886</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="10">
+      <c r="B44" s="10"/>
+      <c r="C44" s="9">
         <v>39878.508333333331</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="10">
+      <c r="D44" s="10"/>
+      <c r="E44" s="9">
         <v>39878.550694444442</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="10">
+      <c r="F44" s="10"/>
+      <c r="G44" s="9">
         <v>39878.800694444442</v>
       </c>
-      <c r="H44" s="11"/>
+      <c r="H44" s="10"/>
       <c r="I44" s="5">
         <f t="shared" si="8"/>
         <v>0.35069444444525288</v>
       </c>
-      <c r="J44" s="11"/>
+      <c r="J44" s="10"/>
       <c r="K44" s="6">
         <f t="shared" si="9"/>
         <v>1.7361111111919569E-2</v>
       </c>
-      <c r="L44" s="11"/>
+      <c r="L44" s="10"/>
       <c r="M44" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="10">
+      <c r="A45" s="9">
         <v>39879.397222222222</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="10">
+      <c r="B45" s="10"/>
+      <c r="C45" s="9">
         <v>39879.51458333333</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="10">
+      <c r="D45" s="10"/>
+      <c r="E45" s="9">
         <v>39879.564583333333</v>
       </c>
-      <c r="F45" s="11"/>
-      <c r="G45" s="10">
+      <c r="F45" s="10"/>
+      <c r="G45" s="9">
         <v>39879.74722222222</v>
       </c>
-      <c r="H45" s="11"/>
+      <c r="H45" s="10"/>
       <c r="I45" s="5">
         <f t="shared" si="8"/>
         <v>0.29999999999563443</v>
       </c>
-      <c r="J45" s="11"/>
+      <c r="J45" s="10"/>
       <c r="K45" s="6">
         <f t="shared" si="9"/>
         <v>-3.3333333337698889E-2</v>
       </c>
-      <c r="L45" s="11"/>
+      <c r="L45" s="10"/>
       <c r="M45" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Sexta</v>
       </c>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="10">
+      <c r="A46" s="12">
         <v>39882.407638888886</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="10">
+      <c r="B46" s="13"/>
+      <c r="C46" s="12">
         <v>39882.51666666667</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="10">
+      <c r="D46" s="13"/>
+      <c r="E46" s="12">
         <v>39882.564583333333</v>
       </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="10">
+      <c r="F46" s="13"/>
+      <c r="G46" s="12">
         <v>39882.875</v>
       </c>
-      <c r="H46" s="11"/>
-      <c r="I46" s="5">
+      <c r="H46" s="13"/>
+      <c r="I46" s="15">
         <f t="shared" si="8"/>
         <v>0.41944444445107365</v>
       </c>
-      <c r="J46" s="11"/>
-      <c r="K46" s="6">
+      <c r="J46" s="13"/>
+      <c r="K46" s="16">
         <f t="shared" si="9"/>
         <v>8.6111111117740335E-2</v>
       </c>
-      <c r="L46" s="11"/>
-      <c r="M46" s="4" t="str">
+      <c r="L46" s="13"/>
+      <c r="M46" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="10">
+      <c r="A47" s="12">
         <v>39883.405555555553</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="10">
+      <c r="B47" s="13"/>
+      <c r="C47" s="12">
         <v>39883.51666666667</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="10">
+      <c r="D47" s="13"/>
+      <c r="E47" s="12">
         <v>39883.565972222219</v>
       </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="10">
+      <c r="F47" s="13"/>
+      <c r="G47" s="12">
         <v>39883.796527777777</v>
       </c>
-      <c r="H47" s="11"/>
-      <c r="I47" s="5">
+      <c r="H47" s="13"/>
+      <c r="I47" s="15">
         <f t="shared" si="8"/>
         <v>0.34166666667442769</v>
       </c>
-      <c r="J47" s="11"/>
-      <c r="K47" s="6">
+      <c r="J47" s="13"/>
+      <c r="K47" s="16">
         <f t="shared" si="9"/>
         <v>8.3333333410943733E-3</v>
       </c>
-      <c r="L47" s="11"/>
-      <c r="M47" s="4" t="str">
+      <c r="L47" s="13"/>
+      <c r="M47" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="10">
+      <c r="A48" s="12">
         <v>39884.40347222222</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="10">
+      <c r="B48" s="13"/>
+      <c r="C48" s="12">
         <v>39884.530555555553</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="10">
+      <c r="D48" s="13"/>
+      <c r="E48" s="12">
         <v>39884.588194444441</v>
       </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="10">
+      <c r="F48" s="13"/>
+      <c r="G48" s="12">
         <v>39884.793749999997</v>
       </c>
-      <c r="H48" s="11"/>
-      <c r="I48" s="5">
+      <c r="H48" s="13"/>
+      <c r="I48" s="15">
         <f t="shared" si="8"/>
         <v>0.33263888888905058</v>
       </c>
-      <c r="J48" s="11"/>
-      <c r="K48" s="6">
+      <c r="J48" s="13"/>
+      <c r="K48" s="16">
         <f t="shared" si="9"/>
         <v>-6.9444444428273799E-4</v>
       </c>
-      <c r="L48" s="11"/>
-      <c r="M48" s="4" t="str">
+      <c r="L48" s="13"/>
+      <c r="M48" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="10">
+      <c r="A49" s="12">
         <v>39885.347222222219</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="10">
+      <c r="B49" s="13"/>
+      <c r="C49" s="12">
         <v>39885.511805555558</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="10">
+      <c r="D49" s="13"/>
+      <c r="E49" s="12">
         <v>39885.560416666667</v>
       </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="10">
+      <c r="F49" s="13"/>
+      <c r="G49" s="12">
         <v>39885.888888888891</v>
       </c>
-      <c r="H49" s="11"/>
-      <c r="I49" s="5">
+      <c r="H49" s="13"/>
+      <c r="I49" s="15">
         <f t="shared" si="8"/>
         <v>0.49305555556202307</v>
       </c>
-      <c r="J49" s="11"/>
-      <c r="K49" s="6">
+      <c r="J49" s="13"/>
+      <c r="K49" s="16">
         <f t="shared" si="9"/>
         <v>0.15972222222868976</v>
       </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="4" t="str">
+      <c r="L49" s="13"/>
+      <c r="M49" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="10">
+      <c r="A50" s="12">
         <v>39886</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="6">
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="16">
         <f t="shared" si="9"/>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="L50" s="11"/>
-      <c r="M50" s="4" t="str">
+      <c r="L50" s="13"/>
+      <c r="M50" s="13" t="str">
         <f t="shared" si="10"/>
         <v>Sexta</v>
       </c>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="10">
+      <c r="A51" s="9">
         <v>39889.413194444445</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="10">
+      <c r="B51" s="10"/>
+      <c r="C51" s="9">
         <v>39889.513888888891</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="10">
+      <c r="D51" s="10"/>
+      <c r="E51" s="9">
         <v>39889.563194444447</v>
       </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="10">
+      <c r="F51" s="10"/>
+      <c r="G51" s="9">
         <v>39889.795138888891</v>
       </c>
-      <c r="H51" s="11"/>
+      <c r="H51" s="10"/>
       <c r="I51" s="5">
         <f t="shared" si="8"/>
         <v>0.33263888888905058</v>
       </c>
-      <c r="J51" s="11"/>
+      <c r="J51" s="10"/>
       <c r="K51" s="6">
         <f t="shared" si="9"/>
         <v>-6.9444444428273799E-4</v>
       </c>
-      <c r="L51" s="11"/>
+      <c r="L51" s="10"/>
       <c r="M51" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="10">
+      <c r="A52" s="9">
         <v>39890.410416666666</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="10">
+      <c r="B52" s="10"/>
+      <c r="C52" s="9">
         <v>39890.515972222223</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="10">
+      <c r="D52" s="10"/>
+      <c r="E52" s="9">
         <v>39890.560416666667</v>
       </c>
-      <c r="F52" s="11"/>
-      <c r="G52" s="10">
+      <c r="F52" s="10"/>
+      <c r="G52" s="9">
         <v>39890.795138888891</v>
       </c>
-      <c r="H52" s="11"/>
+      <c r="H52" s="10"/>
       <c r="I52" s="5">
         <f t="shared" si="8"/>
         <v>0.34027777778101154</v>
       </c>
-      <c r="J52" s="11"/>
+      <c r="J52" s="10"/>
       <c r="K52" s="6">
         <f t="shared" si="9"/>
         <v>6.9444444476782219E-3</v>
       </c>
-      <c r="L52" s="11"/>
+      <c r="L52" s="10"/>
       <c r="M52" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="10">
+      <c r="A53" s="9">
         <v>39891.408333333333</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="10">
+      <c r="B53" s="10"/>
+      <c r="C53" s="9">
         <v>39891.512499999997</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="10">
+      <c r="D53" s="10"/>
+      <c r="E53" s="9">
         <v>39891.5625</v>
       </c>
-      <c r="F53" s="11"/>
-      <c r="G53" s="10">
+      <c r="F53" s="10"/>
+      <c r="G53" s="9">
         <v>39891.792361111111</v>
       </c>
-      <c r="H53" s="11"/>
+      <c r="H53" s="10"/>
       <c r="I53" s="5">
         <f t="shared" si="8"/>
         <v>0.33402777777519077</v>
       </c>
-      <c r="J53" s="11"/>
+      <c r="J53" s="10"/>
       <c r="K53" s="6">
         <f t="shared" si="9"/>
         <v>6.944444418574558E-4</v>
       </c>
-      <c r="L53" s="11"/>
+      <c r="L53" s="10"/>
       <c r="M53" s="4" t="str">
         <f t="shared" si="10"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="10">
+      <c r="A54" s="9">
         <v>39892.408333333333</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="10">
+      <c r="B54" s="10"/>
+      <c r="C54" s="9">
         <v>39892.495138888888</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="10">
+      <c r="D54" s="10"/>
+      <c r="E54" s="9">
         <v>39892.566666666666</v>
       </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="10">
+      <c r="F54" s="10"/>
+      <c r="G54" s="9">
         <v>39892.793055555558</v>
       </c>
-      <c r="H54" s="11"/>
+      <c r="H54" s="10"/>
       <c r="I54" s="5">
-        <f t="shared" ref="I54:I68" si="11">(G54-E54)+(C54-A54)</f>
+        <f t="shared" ref="I54:I77" si="11">(G54-E54)+(C54-A54)</f>
         <v>0.31319444444670808</v>
       </c>
-      <c r="J54" s="11"/>
+      <c r="J54" s="10"/>
       <c r="K54" s="6">
-        <f t="shared" ref="K54:K68" si="12">IF(OR(WEEKDAY(A54)=7,WEEKDAY(A54)=1),I54,I54-"08:00:00")</f>
+        <f t="shared" ref="K54:K77" si="12">IF(OR(WEEKDAY(A54)=7,WEEKDAY(A54)=1),I54,I54-"08:00:00")</f>
         <v>-2.0138888886625239E-2</v>
       </c>
-      <c r="L54" s="11"/>
+      <c r="L54" s="10"/>
       <c r="M54" s="4" t="str">
-        <f t="shared" ref="M54:M68" si="13">IF(WEEKDAY(A54)=1,"Domingo",IF(WEEKDAY(A54)=2,"Segunda",IF(WEEKDAY(A54)=3,"Terça",IF(WEEKDAY(A54)=4,"Quarta",IF(WEEKDAY(A54)=5,"Quinta",IF(WEEKDAY(A54)=6,"Sexta",IF(WEEKDAY(A54)=7,"Sábado","Domingo")))))))</f>
+        <f t="shared" ref="M54:M77" si="13">IF(WEEKDAY(A54)=1,"Domingo",IF(WEEKDAY(A54)=2,"Segunda",IF(WEEKDAY(A54)=3,"Terça",IF(WEEKDAY(A54)=4,"Quarta",IF(WEEKDAY(A54)=5,"Quinta",IF(WEEKDAY(A54)=6,"Sexta",IF(WEEKDAY(A54)=7,"Sábado","Domingo")))))))</f>
         <v>Quinta</v>
       </c>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="10">
+      <c r="A55" s="9">
         <v>39893.338888888888</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="10">
+      <c r="B55" s="10"/>
+      <c r="C55" s="9">
         <v>39893.508333333331</v>
       </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="10">
+      <c r="D55" s="10"/>
+      <c r="E55" s="9">
         <v>39893.546527777777</v>
       </c>
-      <c r="F55" s="11"/>
-      <c r="G55" s="10">
+      <c r="F55" s="10"/>
+      <c r="G55" s="9">
         <v>39893.68472222222</v>
       </c>
-      <c r="H55" s="11"/>
+      <c r="H55" s="10"/>
       <c r="I55" s="5">
         <f t="shared" si="11"/>
         <v>0.30763888888759539</v>
       </c>
-      <c r="J55" s="11"/>
+      <c r="J55" s="10"/>
       <c r="K55" s="6">
         <f t="shared" si="12"/>
         <v>-2.569444444573793E-2</v>
       </c>
-      <c r="L55" s="11"/>
+      <c r="L55" s="10"/>
       <c r="M55" s="4" t="str">
         <f t="shared" si="13"/>
         <v>Sexta</v>
       </c>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="10">
+      <c r="A56" s="12">
         <v>39896.398611111108</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="10">
+      <c r="B56" s="13"/>
+      <c r="C56" s="12">
         <v>39896.510416666664</v>
       </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="10">
+      <c r="D56" s="13"/>
+      <c r="E56" s="12">
         <v>39896.565972222219</v>
       </c>
-      <c r="F56" s="11"/>
-      <c r="G56" s="10">
+      <c r="F56" s="13"/>
+      <c r="G56" s="12">
         <v>39896.782638888886</v>
       </c>
-      <c r="H56" s="11"/>
-      <c r="I56" s="5">
+      <c r="H56" s="13"/>
+      <c r="I56" s="15">
         <f t="shared" si="11"/>
         <v>0.32847222222335404</v>
       </c>
-      <c r="J56" s="11"/>
-      <c r="K56" s="6">
+      <c r="J56" s="13"/>
+      <c r="K56" s="16">
         <f t="shared" si="12"/>
         <v>-4.861111109979277E-3</v>
       </c>
-      <c r="L56" s="11"/>
-      <c r="M56" s="4" t="str">
+      <c r="L56" s="13"/>
+      <c r="M56" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="10">
+      <c r="A57" s="12">
         <v>39897.394444444442</v>
       </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="10">
+      <c r="B57" s="13"/>
+      <c r="C57" s="12">
         <v>39897.518750000003</v>
       </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="10">
+      <c r="D57" s="13"/>
+      <c r="E57" s="12">
         <v>39897.571527777778</v>
       </c>
-      <c r="F57" s="11"/>
-      <c r="G57" s="10">
+      <c r="F57" s="13"/>
+      <c r="G57" s="12">
         <v>39897.776388888888</v>
       </c>
-      <c r="H57" s="11"/>
-      <c r="I57" s="5">
+      <c r="H57" s="13"/>
+      <c r="I57" s="15">
         <f t="shared" si="11"/>
         <v>0.32916666667006211</v>
       </c>
-      <c r="J57" s="11"/>
-      <c r="K57" s="6">
+      <c r="J57" s="13"/>
+      <c r="K57" s="16">
         <f t="shared" si="12"/>
         <v>-4.1666666632712013E-3</v>
       </c>
-      <c r="L57" s="11"/>
-      <c r="M57" s="4" t="str">
+      <c r="L57" s="13"/>
+      <c r="M57" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="10">
+      <c r="A58" s="12">
         <v>39898.401388888888</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="10">
+      <c r="B58" s="13"/>
+      <c r="C58" s="12">
         <v>39898.519444444442</v>
       </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10">
+      <c r="D58" s="13"/>
+      <c r="E58" s="12">
         <v>39898.579861111109</v>
       </c>
-      <c r="F58" s="11"/>
-      <c r="G58" s="10">
+      <c r="F58" s="13"/>
+      <c r="G58" s="12">
         <v>39898.799305555556</v>
       </c>
-      <c r="H58" s="11"/>
-      <c r="I58" s="5">
+      <c r="H58" s="13"/>
+      <c r="I58" s="15">
         <f t="shared" si="11"/>
         <v>0.33750000000145519</v>
       </c>
-      <c r="J58" s="11"/>
-      <c r="K58" s="6">
+      <c r="J58" s="13"/>
+      <c r="K58" s="16">
         <f t="shared" si="12"/>
         <v>4.1666666681218767E-3</v>
       </c>
-      <c r="L58" s="11"/>
-      <c r="M58" s="4" t="str">
+      <c r="L58" s="13"/>
+      <c r="M58" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="10">
+      <c r="A59" s="12">
         <v>39899.319444444445</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="10">
+      <c r="B59" s="13"/>
+      <c r="C59" s="12">
         <v>39899.513888888891</v>
       </c>
-      <c r="D59" s="11"/>
-      <c r="E59" s="10">
+      <c r="D59" s="13"/>
+      <c r="E59" s="12">
         <v>39899.554166666669</v>
       </c>
-      <c r="F59" s="11"/>
-      <c r="G59" s="10">
+      <c r="F59" s="13"/>
+      <c r="G59" s="12">
         <v>39899.697916666664</v>
       </c>
-      <c r="H59" s="11"/>
-      <c r="I59" s="5">
+      <c r="H59" s="13"/>
+      <c r="I59" s="15">
         <f t="shared" si="11"/>
         <v>0.33819444444088731</v>
       </c>
-      <c r="J59" s="11"/>
-      <c r="K59" s="6">
+      <c r="J59" s="13"/>
+      <c r="K59" s="16">
         <f t="shared" si="12"/>
         <v>4.8611111075539948E-3</v>
       </c>
-      <c r="L59" s="11"/>
-      <c r="M59" s="4" t="str">
+      <c r="L59" s="13"/>
+      <c r="M59" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="10">
+      <c r="A60" s="9">
         <v>39903.402083333334</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="10">
+      <c r="B60" s="10"/>
+      <c r="C60" s="9">
         <v>39903.509722222225</v>
       </c>
-      <c r="D60" s="11"/>
-      <c r="E60" s="10">
+      <c r="D60" s="10"/>
+      <c r="E60" s="9">
         <v>39903.551388888889</v>
       </c>
-      <c r="F60" s="11"/>
-      <c r="G60" s="10">
+      <c r="F60" s="10"/>
+      <c r="G60" s="9">
         <v>39903.805555555555</v>
       </c>
-      <c r="H60" s="11"/>
+      <c r="H60" s="10"/>
       <c r="I60" s="5">
         <f t="shared" si="11"/>
         <v>0.36180555555620231</v>
       </c>
-      <c r="J60" s="11"/>
+      <c r="J60" s="10"/>
       <c r="K60" s="6">
         <f t="shared" si="12"/>
         <v>2.8472222222868993E-2</v>
       </c>
-      <c r="L60" s="11"/>
+      <c r="L60" s="10"/>
       <c r="M60" s="4" t="str">
         <f t="shared" si="13"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="10">
+      <c r="A61" s="9">
         <v>39904.404166666667</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="10">
+      <c r="B61" s="10"/>
+      <c r="C61" s="9">
         <v>39904.511111111111</v>
       </c>
-      <c r="D61" s="11"/>
-      <c r="E61" s="10">
+      <c r="D61" s="10"/>
+      <c r="E61" s="9">
         <v>39904.544444444444</v>
       </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="10">
+      <c r="F61" s="10"/>
+      <c r="G61" s="9">
         <v>39904.854861111111</v>
       </c>
-      <c r="H61" s="11"/>
+      <c r="H61" s="10"/>
       <c r="I61" s="5">
         <f t="shared" si="11"/>
         <v>0.41736111111094942</v>
       </c>
-      <c r="J61" s="11"/>
+      <c r="J61" s="10"/>
       <c r="K61" s="6">
         <f t="shared" si="12"/>
         <v>8.4027777777616108E-2</v>
       </c>
-      <c r="L61" s="11"/>
+      <c r="L61" s="10"/>
       <c r="M61" s="4" t="str">
         <f t="shared" si="13"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="10">
+      <c r="A62" s="9">
         <v>39905.40902777778</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="10">
+      <c r="B62" s="10"/>
+      <c r="C62" s="9">
         <v>39905.526388888888</v>
       </c>
-      <c r="D62" s="11"/>
-      <c r="E62" s="10">
+      <c r="D62" s="10"/>
+      <c r="E62" s="9">
         <v>39905.570833333331</v>
       </c>
-      <c r="F62" s="11"/>
-      <c r="G62" s="10">
+      <c r="F62" s="10"/>
+      <c r="G62" s="9">
         <v>39905.836805555555</v>
       </c>
-      <c r="H62" s="11"/>
+      <c r="H62" s="10"/>
       <c r="I62" s="5">
         <f t="shared" si="11"/>
         <v>0.38333333333139308</v>
       </c>
-      <c r="J62" s="11"/>
+      <c r="J62" s="10"/>
       <c r="K62" s="6">
         <f t="shared" si="12"/>
         <v>4.9999999998059763E-2</v>
       </c>
-      <c r="L62" s="11"/>
+      <c r="L62" s="10"/>
       <c r="M62" s="4" t="str">
         <f t="shared" si="13"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="10">
+      <c r="A63" s="9">
         <v>39906.408333333333</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="10">
+      <c r="B63" s="10"/>
+      <c r="C63" s="9">
         <v>39906.518750000003</v>
       </c>
-      <c r="D63" s="11"/>
-      <c r="E63" s="10">
+      <c r="D63" s="10"/>
+      <c r="E63" s="9">
         <v>39906.563888888886</v>
       </c>
-      <c r="F63" s="11"/>
-      <c r="G63" s="10">
+      <c r="F63" s="10"/>
+      <c r="G63" s="9">
         <v>39906.830555555556</v>
       </c>
-      <c r="H63" s="11"/>
+      <c r="H63" s="10"/>
       <c r="I63" s="5">
         <f t="shared" si="11"/>
         <v>0.37708333334012423</v>
       </c>
-      <c r="J63" s="11"/>
+      <c r="J63" s="10"/>
       <c r="K63" s="6">
         <f t="shared" si="12"/>
         <v>4.3750000006790912E-2</v>
       </c>
-      <c r="L63" s="11"/>
+      <c r="L63" s="10"/>
       <c r="M63" s="4" t="str">
         <f t="shared" si="13"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="10">
+      <c r="A64" s="9">
         <v>39907.327777777777</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="10">
+      <c r="B64" s="10"/>
+      <c r="C64" s="9">
         <v>39907.522222222222</v>
       </c>
-      <c r="D64" s="11"/>
-      <c r="E64" s="10">
+      <c r="D64" s="10"/>
+      <c r="E64" s="9">
         <v>39907.565972222219</v>
       </c>
-      <c r="F64" s="11"/>
-      <c r="G64" s="10">
+      <c r="F64" s="10"/>
+      <c r="G64" s="9">
         <v>39907.717361111114</v>
       </c>
-      <c r="H64" s="11"/>
+      <c r="H64" s="10"/>
       <c r="I64" s="5">
         <f t="shared" si="11"/>
         <v>0.34583333334012423</v>
       </c>
-      <c r="J64" s="11"/>
+      <c r="J64" s="10"/>
       <c r="K64" s="6">
         <f t="shared" si="12"/>
         <v>1.2500000006790912E-2</v>
       </c>
-      <c r="L64" s="11"/>
+      <c r="L64" s="10"/>
       <c r="M64" s="4" t="str">
         <f t="shared" si="13"/>
         <v>Sexta</v>
       </c>
     </row>
     <row r="65" spans="1:13">
-      <c r="A65" s="10">
+      <c r="A65" s="12">
         <v>39910.405555555553</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="10">
+      <c r="B65" s="13"/>
+      <c r="C65" s="12">
         <v>39910.51666666667</v>
       </c>
-      <c r="D65" s="11"/>
-      <c r="E65" s="10">
+      <c r="D65" s="13"/>
+      <c r="E65" s="12">
         <v>39910.559027777781</v>
       </c>
-      <c r="F65" s="11"/>
-      <c r="G65" s="10">
+      <c r="F65" s="13"/>
+      <c r="G65" s="12">
         <v>39910.844444444447</v>
       </c>
-      <c r="H65" s="11"/>
-      <c r="I65" s="5">
+      <c r="H65" s="13"/>
+      <c r="I65" s="15">
         <f t="shared" si="11"/>
         <v>0.39652777778246673</v>
       </c>
-      <c r="J65" s="11"/>
-      <c r="K65" s="6">
+      <c r="J65" s="13"/>
+      <c r="K65" s="16">
         <f t="shared" si="12"/>
         <v>6.3194444449133413E-2</v>
       </c>
-      <c r="L65" s="11"/>
-      <c r="M65" s="4" t="str">
+      <c r="L65" s="13"/>
+      <c r="M65" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Segunda</v>
       </c>
     </row>
     <row r="66" spans="1:13">
-      <c r="A66" s="10">
+      <c r="A66" s="12">
         <v>39911.404166666667</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="10">
+      <c r="B66" s="13"/>
+      <c r="C66" s="12">
         <v>39911.520138888889</v>
       </c>
-      <c r="D66" s="11"/>
-      <c r="E66" s="10">
+      <c r="D66" s="13"/>
+      <c r="E66" s="12">
         <v>39911.561111111114</v>
       </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="10">
+      <c r="F66" s="13"/>
+      <c r="G66" s="12">
         <v>39911.842361111114</v>
       </c>
-      <c r="H66" s="11"/>
-      <c r="I66" s="5">
+      <c r="H66" s="13"/>
+      <c r="I66" s="15">
         <f t="shared" si="11"/>
         <v>0.39722222222189885</v>
       </c>
-      <c r="J66" s="11"/>
-      <c r="K66" s="6">
+      <c r="J66" s="13"/>
+      <c r="K66" s="16">
         <f t="shared" si="12"/>
         <v>6.3888888888565531E-2</v>
       </c>
-      <c r="L66" s="11"/>
-      <c r="M66" s="4" t="str">
+      <c r="L66" s="13"/>
+      <c r="M66" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Terça</v>
       </c>
     </row>
     <row r="67" spans="1:13">
-      <c r="A67" s="10">
+      <c r="A67" s="12">
         <v>39912.402083333334</v>
       </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="10">
+      <c r="B67" s="13"/>
+      <c r="C67" s="12">
         <v>39912.519444444442</v>
       </c>
-      <c r="D67" s="11"/>
-      <c r="E67" s="10">
+      <c r="D67" s="13"/>
+      <c r="E67" s="12">
         <v>39912.56527777778</v>
       </c>
-      <c r="F67" s="11"/>
-      <c r="G67" s="10">
+      <c r="F67" s="13"/>
+      <c r="G67" s="12">
         <v>39912.804166666669</v>
       </c>
-      <c r="H67" s="11"/>
-      <c r="I67" s="5">
+      <c r="H67" s="13"/>
+      <c r="I67" s="15">
         <f t="shared" si="11"/>
         <v>0.35624999999708962</v>
       </c>
-      <c r="J67" s="11"/>
-      <c r="K67" s="6">
+      <c r="J67" s="13"/>
+      <c r="K67" s="16">
         <f t="shared" si="12"/>
         <v>2.2916666663756302E-2</v>
       </c>
-      <c r="L67" s="11"/>
-      <c r="M67" s="4" t="str">
+      <c r="L67" s="13"/>
+      <c r="M67" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Quarta</v>
       </c>
     </row>
     <row r="68" spans="1:13">
-      <c r="A68" s="10">
+      <c r="A68" s="12">
         <v>39913.401388888888</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="10">
+      <c r="B68" s="13"/>
+      <c r="C68" s="12">
         <v>39913.524305555555</v>
       </c>
-      <c r="D68" s="11"/>
-      <c r="E68" s="10">
+      <c r="D68" s="13"/>
+      <c r="E68" s="12">
         <v>39913.600694444445</v>
       </c>
-      <c r="F68" s="11"/>
-      <c r="G68" s="10">
+      <c r="F68" s="13"/>
+      <c r="G68" s="12">
         <v>39913.838888888888</v>
       </c>
-      <c r="H68" s="11"/>
-      <c r="I68" s="5">
+      <c r="H68" s="13"/>
+      <c r="I68" s="15">
         <f t="shared" si="11"/>
         <v>0.36111111110949423</v>
       </c>
-      <c r="J68" s="11"/>
-      <c r="K68" s="6">
+      <c r="J68" s="13"/>
+      <c r="K68" s="16">
         <f t="shared" si="12"/>
         <v>2.7777777776160917E-2</v>
       </c>
-      <c r="L68" s="11"/>
-      <c r="M68" s="4" t="str">
+      <c r="L68" s="13"/>
+      <c r="M68" s="13" t="str">
         <f t="shared" si="13"/>
         <v>Quinta</v>
       </c>
     </row>
     <row r="69" spans="1:13">
-      <c r="B69" s="12"/>
+      <c r="A69" s="12">
+        <v>39914.323611111111</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="12">
+        <v>39914.515972222223</v>
+      </c>
+      <c r="D69" s="13"/>
+      <c r="E69" s="12">
+        <v>39914.561111111114</v>
+      </c>
+      <c r="F69" s="13"/>
+      <c r="G69" s="12">
+        <v>39914.701388888891</v>
+      </c>
+      <c r="H69" s="13"/>
+      <c r="I69" s="15">
+        <f t="shared" si="11"/>
+        <v>0.33263888888905058</v>
+      </c>
+      <c r="J69" s="13"/>
+      <c r="K69" s="16">
+        <f t="shared" si="12"/>
+        <v>-6.9444444428273799E-4</v>
+      </c>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>Sexta</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" s="9">
+        <v>39917.460416666669</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="9">
+        <v>39917.519444444442</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="E70" s="9">
+        <v>39917.568055555559</v>
+      </c>
+      <c r="F70" s="10"/>
+      <c r="G70" s="9">
+        <v>39917.852083333331</v>
+      </c>
+      <c r="H70" s="10"/>
+      <c r="I70" s="5">
+        <f t="shared" si="11"/>
+        <v>0.34305555554601597</v>
+      </c>
+      <c r="J70" s="10"/>
+      <c r="K70" s="6">
+        <f t="shared" si="12"/>
+        <v>9.7222222126826519E-3</v>
+      </c>
+      <c r="L70" s="10"/>
+      <c r="M70" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>Segunda</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="9">
+        <v>39918.399305555555</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="9">
+        <v>39918.520138888889</v>
+      </c>
+      <c r="D71" s="10"/>
+      <c r="E71" s="9">
+        <v>39918.565972222219</v>
+      </c>
+      <c r="F71" s="10"/>
+      <c r="G71" s="9">
+        <v>39918.786805555559</v>
+      </c>
+      <c r="H71" s="10"/>
+      <c r="I71" s="5">
+        <f t="shared" si="11"/>
+        <v>0.34166666667442769</v>
+      </c>
+      <c r="J71" s="10"/>
+      <c r="K71" s="6">
+        <f t="shared" si="12"/>
+        <v>8.3333333410943733E-3</v>
+      </c>
+      <c r="L71" s="10"/>
+      <c r="M71" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>Terça</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="9">
+        <v>39919.395833333336</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="9">
+        <v>39919.520138888889</v>
+      </c>
+      <c r="D72" s="10"/>
+      <c r="E72" s="9">
+        <v>39919.561111111114</v>
+      </c>
+      <c r="F72" s="10"/>
+      <c r="G72" s="9">
+        <v>39919.777777777781</v>
+      </c>
+      <c r="H72" s="10"/>
+      <c r="I72" s="5">
+        <f t="shared" si="11"/>
+        <v>0.34097222222044365</v>
+      </c>
+      <c r="J72" s="10"/>
+      <c r="K72" s="6">
+        <f t="shared" si="12"/>
+        <v>7.63888888711034E-3</v>
+      </c>
+      <c r="L72" s="10"/>
+      <c r="M72" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>Quarta</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="9">
+        <v>39920.415972222225</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="9">
+        <v>39920.561111111114</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" s="9">
+        <v>39920.597916666666</v>
+      </c>
+      <c r="F73" s="10"/>
+      <c r="G73" s="9">
+        <v>39920.795138888891</v>
+      </c>
+      <c r="H73" s="10"/>
+      <c r="I73" s="5">
+        <f t="shared" si="11"/>
+        <v>0.34236111111385981</v>
+      </c>
+      <c r="J73" s="10"/>
+      <c r="K73" s="6">
+        <f t="shared" si="12"/>
+        <v>9.0277777805264914E-3</v>
+      </c>
+      <c r="L73" s="10"/>
+      <c r="M73" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>Quinta</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="9">
+        <v>39921.326388888891</v>
+      </c>
+      <c r="B74" s="10"/>
+      <c r="C74" s="9">
+        <v>39921.505555555559</v>
+      </c>
+      <c r="D74" s="10"/>
+      <c r="E74" s="9">
+        <v>39921.547222222223</v>
+      </c>
+      <c r="F74" s="10"/>
+      <c r="G74" s="9">
+        <v>39921.693055555559</v>
+      </c>
+      <c r="H74" s="10"/>
+      <c r="I74" s="5">
+        <f t="shared" si="11"/>
+        <v>0.32500000000436557</v>
+      </c>
+      <c r="J74" s="10"/>
+      <c r="K74" s="6">
+        <f t="shared" si="12"/>
+        <v>-8.3333333289677403E-3</v>
+      </c>
+      <c r="L74" s="10"/>
+      <c r="M74" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>Sexta</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="12">
+        <v>39924.40625</v>
+      </c>
+      <c r="B75" s="13"/>
+      <c r="C75" s="12">
+        <v>39924.523611111108</v>
+      </c>
+      <c r="D75" s="13"/>
+      <c r="E75" s="12">
+        <v>39924.563888888886</v>
+      </c>
+      <c r="F75" s="13"/>
+      <c r="G75" s="12">
+        <v>39924.784722222219</v>
+      </c>
+      <c r="H75" s="13"/>
+      <c r="I75" s="15">
+        <f t="shared" si="11"/>
+        <v>0.33819444444088731</v>
+      </c>
+      <c r="J75" s="13"/>
+      <c r="K75" s="16">
+        <f t="shared" si="12"/>
+        <v>4.8611111075539948E-3</v>
+      </c>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>Segunda</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="12">
+        <v>39925.397916666669</v>
+      </c>
+      <c r="B76" s="13"/>
+      <c r="C76" s="12">
+        <v>39925.504166666666</v>
+      </c>
+      <c r="D76" s="13"/>
+      <c r="E76" s="12">
+        <v>39925.545138888891</v>
+      </c>
+      <c r="F76" s="13"/>
+      <c r="G76" s="12">
+        <v>39925.772916666669</v>
+      </c>
+      <c r="H76" s="13"/>
+      <c r="I76" s="15">
+        <f t="shared" si="11"/>
+        <v>0.33402777777519077</v>
+      </c>
+      <c r="J76" s="13"/>
+      <c r="K76" s="16">
+        <f t="shared" si="12"/>
+        <v>6.944444418574558E-4</v>
+      </c>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>Terça</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="12">
+        <v>39926.375</v>
+      </c>
+      <c r="B77" s="13"/>
+      <c r="C77" s="12">
+        <v>39926.517361111109</v>
+      </c>
+      <c r="D77" s="13"/>
+      <c r="E77" s="12">
+        <v>39926.565972222219</v>
+      </c>
+      <c r="F77" s="13"/>
+      <c r="G77" s="12">
+        <v>39926.754861111112</v>
+      </c>
+      <c r="H77" s="13"/>
+      <c r="I77" s="15">
+        <f t="shared" si="11"/>
+        <v>0.33125000000291038</v>
+      </c>
+      <c r="J77" s="13"/>
+      <c r="K77" s="16">
+        <f t="shared" si="12"/>
+        <v>-2.0833333304229318E-3</v>
+      </c>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>Quarta</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="B78" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>